<commit_message>
optomized runtime and getting a variety of solutions from the total pool
</commit_message>
<xml_diff>
--- a/selected_solutions.xlsx
+++ b/selected_solutions.xlsx
@@ -19,6 +19,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O_2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O_2y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O_4x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O_4y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W + V1 + U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THETA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BETA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAMMA2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -29,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:S2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -121,6 +202,83 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2.583857651108</v>

</xml_diff>